<commit_message>
Update Files and Location
</commit_message>
<xml_diff>
--- a/Excel_Practice_Student.xlsx
+++ b/Excel_Practice_Student.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamr\Code\SavvyCoders\Activities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B79D389-BA62-4701-9CEC-AB828EFC8801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCABE001-1970-4F55-9BCA-6CB934F8CDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8D4C5268-695D-4616-9E91-53744754ABC6}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8D4C5268-695D-4616-9E91-53744754ABC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -943,7 +943,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -988,9 +988,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3713,7 +3710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5AA2E7-F047-42D2-AD6F-D303D1F75E1A}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -3860,8 +3857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB70C1B-75BF-4BA5-9170-95D94596A40F}">
   <dimension ref="A1:N240"/>
   <sheetViews>
-    <sheetView topLeftCell="A274" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H92" sqref="H92"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3883,18 +3880,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="F1" s="39" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="F1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -3932,8 +3929,8 @@
       <c r="C3" s="5">
         <v>45</v>
       </c>
-      <c r="D3" s="5" t="b" cm="1">
-        <f t="array" ref="D3">AND(B3:B11="Fire",C3:C11&lt;70)</f>
+      <c r="D3" s="5" t="b">
+        <f>AND(B3="Fire",C3&gt;70)</f>
         <v>0</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -3960,8 +3957,8 @@
       <c r="C4" s="5">
         <v>60</v>
       </c>
-      <c r="D4" s="5" t="b" cm="1">
-        <f t="array" ref="D4">AND(B4:B12="Fire",C4:C12&lt;70)</f>
+      <c r="D4" s="5" t="b">
+        <f t="shared" ref="D4:D11" si="0">AND(B4="Fire",C4&gt;70)</f>
         <v>0</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -3974,7 +3971,7 @@
         <v>60</v>
       </c>
       <c r="I4" s="5" t="str">
-        <f t="shared" ref="I4:I11" si="0">IF(AND(G4="Fire",H4&gt;70), "True", "False")</f>
+        <f t="shared" ref="I4:I11" si="1">IF(AND(G4="Fire",H4&gt;70), "True", "False")</f>
         <v>False</v>
       </c>
     </row>
@@ -3988,8 +3985,8 @@
       <c r="C5" s="5">
         <v>80</v>
       </c>
-      <c r="D5" s="5" t="b" cm="1">
-        <f t="array" ref="D5">AND(B5:B13="Fire",C5:C13&lt;70)</f>
+      <c r="D5" s="5" t="b">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -4002,7 +3999,7 @@
         <v>80</v>
       </c>
       <c r="I5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
     </row>
@@ -4016,8 +4013,8 @@
       <c r="C6" s="5">
         <v>65</v>
       </c>
-      <c r="D6" s="5" t="b" cm="1">
-        <f t="array" ref="D6">AND(B6:B14="Fire",C6:C14&lt;70)</f>
+      <c r="D6" s="5" t="b">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -4030,7 +4027,7 @@
         <v>65</v>
       </c>
       <c r="I6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
     </row>
@@ -4044,9 +4041,9 @@
       <c r="C7" s="5">
         <v>80</v>
       </c>
-      <c r="D7" s="5" t="b" cm="1">
-        <f t="array" ref="D7">AND(B7:B15="Fire",C7:C15&lt;70)</f>
-        <v>0</v>
+      <c r="D7" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>22</v>
@@ -4058,7 +4055,7 @@
         <v>80</v>
       </c>
       <c r="I7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
     </row>
@@ -4072,9 +4069,9 @@
       <c r="C8" s="5">
         <v>100</v>
       </c>
-      <c r="D8" s="5" t="b" cm="1">
-        <f t="array" ref="D8">AND(B8:B16="Fire",C8:C16&lt;70)</f>
-        <v>0</v>
+      <c r="D8" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>23</v>
@@ -4086,7 +4083,7 @@
         <v>100</v>
       </c>
       <c r="I8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
     </row>
@@ -4100,8 +4097,8 @@
       <c r="C9" s="5">
         <v>43</v>
       </c>
-      <c r="D9" s="5" t="b" cm="1">
-        <f t="array" ref="D9">AND(B9:B17="Fire",C9:C17&lt;70)</f>
+      <c r="D9" s="5" t="b">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -4114,7 +4111,7 @@
         <v>43</v>
       </c>
       <c r="I9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
     </row>
@@ -4128,8 +4125,8 @@
       <c r="C10" s="5">
         <v>58</v>
       </c>
-      <c r="D10" s="5" t="b" cm="1">
-        <f t="array" ref="D10">AND(B10:B18="Fire",C10:C18&lt;70)</f>
+      <c r="D10" s="5" t="b">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -4142,7 +4139,7 @@
         <v>58</v>
       </c>
       <c r="I10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
     </row>
@@ -4156,8 +4153,8 @@
       <c r="C11" s="5">
         <v>78</v>
       </c>
-      <c r="D11" s="5" t="b" cm="1">
-        <f t="array" ref="D11">AND(B11:B19="Fire",C11:C19&lt;70)</f>
+      <c r="D11" s="5" t="b">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -4170,7 +4167,7 @@
         <v>78</v>
       </c>
       <c r="I11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
     </row>
@@ -4180,13 +4177,13 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -4261,7 +4258,7 @@
         <v>21</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" ref="E18:E19" si="1">AVERAGEIF($B$15:$B$23,D18,$C$15:$C$23)</f>
+        <f t="shared" ref="E18:E19" si="2">AVERAGEIF($B$15:$B$23,D18,$C$15:$C$23)</f>
         <v>81.666666666666671</v>
       </c>
     </row>
@@ -4279,7 +4276,7 @@
         <v>25</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>59.666666666666664</v>
       </c>
     </row>
@@ -4332,17 +4329,17 @@
       <c r="D23" s="7"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -4401,6 +4398,10 @@
       <c r="G28" s="14">
         <v>1</v>
       </c>
+      <c r="H28" s="4">
+        <f>AVERAGEIFS(C27:C38,B27:B38,"Grass",D27:D38,1)</f>
+        <v>65</v>
+      </c>
       <c r="I28" s="15"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -4422,6 +4423,10 @@
       <c r="G29" s="14">
         <v>1</v>
       </c>
+      <c r="H29" s="4">
+        <f>AVERAGEIFS(C28:C39,B28:B39,"Fire",D28:D39,1)</f>
+        <v>59.666666666666664</v>
+      </c>
       <c r="I29" s="15"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -4443,6 +4448,10 @@
       <c r="G30" s="14">
         <v>2</v>
       </c>
+      <c r="H30" s="4">
+        <f>AVERAGEIFS(C29:C40,B29:B40,"Grass",D29:D40,2)</f>
+        <v>81.666666666666671</v>
+      </c>
       <c r="I30" s="15"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -4464,8 +4473,11 @@
       <c r="G31" s="17">
         <v>2</v>
       </c>
-      <c r="H31" s="18"/>
-      <c r="I31" s="19"/>
+      <c r="H31" s="4">
+        <f>AVERAGEIFS(C30:C41,B30:B41,"Fire",D30:D41,2)</f>
+        <v>59.666666666666664</v>
+      </c>
+      <c r="I31" s="18"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
@@ -4571,18 +4583,18 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="F40" s="38" t="s">
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="F40" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G40" s="38"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="38"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
@@ -5109,18 +5121,18 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="38" t="s">
+      <c r="A64" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="B64" s="38"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
-      <c r="F64" s="39" t="s">
+      <c r="B64" s="37"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
+      <c r="F64" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="G64" s="39"/>
-      <c r="H64" s="39"/>
-      <c r="I64" s="39"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
@@ -5247,7 +5259,7 @@
       <c r="I69" s="5">
         <v>335</v>
       </c>
-      <c r="K69" s="20" t="s">
+      <c r="K69" s="19" t="s">
         <v>17</v>
       </c>
       <c r="L69" s="5">
@@ -5280,11 +5292,11 @@
       <c r="I70" s="5">
         <v>465</v>
       </c>
-      <c r="K70" s="20" t="s">
+      <c r="K70" s="19" t="s">
         <v>25</v>
       </c>
       <c r="L70" s="5">
-        <f t="shared" ref="L70:L79" si="2">COUNTIF(G67:G86,K70)</f>
+        <f t="shared" ref="L70:L79" si="3">COUNTIF(G67:G86,K70)</f>
         <v>6</v>
       </c>
     </row>
@@ -5313,11 +5325,11 @@
       <c r="I71" s="5">
         <v>475</v>
       </c>
-      <c r="K71" s="20" t="s">
+      <c r="K71" s="19" t="s">
         <v>60</v>
       </c>
       <c r="L71" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5346,11 +5358,11 @@
       <c r="I72" s="5">
         <v>525</v>
       </c>
-      <c r="K72" s="20" t="s">
+      <c r="K72" s="19" t="s">
         <v>54</v>
       </c>
       <c r="L72" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5379,11 +5391,11 @@
       <c r="I73" s="5">
         <v>385</v>
       </c>
-      <c r="K73" s="20" t="s">
+      <c r="K73" s="19" t="s">
         <v>66</v>
       </c>
       <c r="L73" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5408,11 +5420,11 @@
       <c r="I74" s="5">
         <v>420</v>
       </c>
-      <c r="K74" s="20" t="s">
+      <c r="K74" s="19" t="s">
         <v>69</v>
       </c>
       <c r="L74" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5441,11 +5453,11 @@
       <c r="I75" s="5">
         <v>349</v>
       </c>
-      <c r="K75" s="20" t="s">
+      <c r="K75" s="19" t="s">
         <v>71</v>
       </c>
       <c r="L75" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -5470,11 +5482,11 @@
       <c r="I76" s="5">
         <v>253</v>
       </c>
-      <c r="K76" s="20" t="s">
+      <c r="K76" s="19" t="s">
         <v>75</v>
       </c>
       <c r="L76" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5503,11 +5515,11 @@
       <c r="I77" s="5">
         <v>395</v>
       </c>
-      <c r="K77" s="20" t="s">
+      <c r="K77" s="19" t="s">
         <v>57</v>
       </c>
       <c r="L77" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -5536,11 +5548,11 @@
       <c r="I78" s="5">
         <v>310</v>
       </c>
-      <c r="K78" s="20" t="s">
+      <c r="K78" s="19" t="s">
         <v>21</v>
       </c>
       <c r="L78" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5565,11 +5577,11 @@
       <c r="I79" s="5">
         <v>475</v>
       </c>
-      <c r="K79" s="20" t="s">
+      <c r="K79" s="19" t="s">
         <v>82</v>
       </c>
       <c r="L79" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5723,16 +5735,16 @@
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="38" t="s">
+      <c r="A88" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="B88" s="38"/>
-      <c r="C88" s="38"/>
-      <c r="D88" s="38"/>
-      <c r="E88" s="38"/>
-      <c r="F88" s="38"/>
-      <c r="G88" s="38"/>
-      <c r="H88" s="38"/>
+      <c r="B88" s="37"/>
+      <c r="C88" s="37"/>
+      <c r="D88" s="37"/>
+      <c r="E88" s="37"/>
+      <c r="F88" s="37"/>
+      <c r="G88" s="37"/>
+      <c r="H88" s="37"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
@@ -5829,7 +5841,7 @@
         <v>2</v>
       </c>
       <c r="H93" s="15">
-        <f t="shared" ref="H93:H95" si="3">COUNTIFS(B91:B102,F93,D91:D102,G93)</f>
+        <f t="shared" ref="H93:H95" si="4">COUNTIFS(B91:B102,F93,D91:D102,G93)</f>
         <v>3</v>
       </c>
     </row>
@@ -5853,7 +5865,7 @@
         <v>1</v>
       </c>
       <c r="H94" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -5877,7 +5889,7 @@
         <v>2</v>
       </c>
       <c r="H95" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -5966,18 +5978,18 @@
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="38" t="s">
+      <c r="A103" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="B103" s="38"/>
-      <c r="C103" s="38"/>
-      <c r="D103" s="38"/>
-      <c r="F103" s="38" t="s">
+      <c r="B103" s="37"/>
+      <c r="C103" s="37"/>
+      <c r="D103" s="37"/>
+      <c r="F103" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="G103" s="38"/>
-      <c r="H103" s="38"/>
-      <c r="I103" s="38"/>
+      <c r="G103" s="37"/>
+      <c r="H103" s="37"/>
+      <c r="I103" s="37"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
@@ -6029,7 +6041,7 @@
         <v>318</v>
       </c>
       <c r="I105" s="4" t="str">
-        <f>IF(H105&gt;"500","Yes","No")</f>
+        <f>IF(H105&gt;500, "Yes", "No")</f>
         <v>No</v>
       </c>
     </row>
@@ -6044,7 +6056,7 @@
         <v>405</v>
       </c>
       <c r="D106" s="4" t="str">
-        <f t="shared" ref="D106:D113" si="4">IF(B106="Grass","Yes","No")</f>
+        <f t="shared" ref="D106:D113" si="5">IF(B106="Grass","Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="F106" s="4" t="s">
@@ -6057,7 +6069,7 @@
         <v>405</v>
       </c>
       <c r="I106" s="4" t="str">
-        <f t="shared" ref="I106:I113" si="5">IF(H106&gt;"500","Yes","No")</f>
+        <f t="shared" ref="I106:I113" si="6">IF(H106&gt;500, "Yes", "No")</f>
         <v>No</v>
       </c>
     </row>
@@ -6072,7 +6084,7 @@
         <v>525</v>
       </c>
       <c r="D107" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Yes</v>
       </c>
       <c r="F107" s="4" t="s">
@@ -6085,8 +6097,8 @@
         <v>525</v>
       </c>
       <c r="I107" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>No</v>
+        <f t="shared" si="6"/>
+        <v>Yes</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -6100,7 +6112,7 @@
         <v>309</v>
       </c>
       <c r="D108" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>No</v>
       </c>
       <c r="F108" s="4" t="s">
@@ -6113,7 +6125,7 @@
         <v>309</v>
       </c>
       <c r="I108" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>No</v>
       </c>
     </row>
@@ -6128,7 +6140,7 @@
         <v>405</v>
       </c>
       <c r="D109" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>No</v>
       </c>
       <c r="F109" s="4" t="s">
@@ -6141,7 +6153,7 @@
         <v>405</v>
       </c>
       <c r="I109" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>No</v>
       </c>
     </row>
@@ -6156,7 +6168,7 @@
         <v>534</v>
       </c>
       <c r="D110" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>No</v>
       </c>
       <c r="F110" s="4" t="s">
@@ -6169,8 +6181,8 @@
         <v>534</v>
       </c>
       <c r="I110" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>No</v>
+        <f t="shared" si="6"/>
+        <v>Yes</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -6184,7 +6196,7 @@
         <v>314</v>
       </c>
       <c r="D111" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>No</v>
       </c>
       <c r="F111" s="4" t="s">
@@ -6197,7 +6209,7 @@
         <v>314</v>
       </c>
       <c r="I111" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>No</v>
       </c>
     </row>
@@ -6212,7 +6224,7 @@
         <v>405</v>
       </c>
       <c r="D112" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>No</v>
       </c>
       <c r="F112" s="4" t="s">
@@ -6225,7 +6237,7 @@
         <v>405</v>
       </c>
       <c r="I112" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>No</v>
       </c>
     </row>
@@ -6240,7 +6252,7 @@
         <v>530</v>
       </c>
       <c r="D113" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>No</v>
       </c>
       <c r="F113" s="4" t="s">
@@ -6253,8 +6265,8 @@
         <v>530</v>
       </c>
       <c r="I113" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>No</v>
+        <f t="shared" si="6"/>
+        <v>Yes</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
@@ -6266,21 +6278,21 @@
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A115" s="38" t="s">
+      <c r="A115" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="B115" s="38"/>
-      <c r="C115" s="38"/>
-      <c r="D115" s="38"/>
-      <c r="F115" s="38" t="s">
+      <c r="B115" s="37"/>
+      <c r="C115" s="37"/>
+      <c r="D115" s="37"/>
+      <c r="F115" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="G115" s="38"/>
-      <c r="H115" s="38"/>
-      <c r="I115" s="38"/>
-      <c r="J115" s="38"/>
-      <c r="K115" s="38"/>
-      <c r="L115" s="38"/>
+      <c r="G115" s="37"/>
+      <c r="H115" s="37"/>
+      <c r="I115" s="37"/>
+      <c r="J115" s="37"/>
+      <c r="K115" s="37"/>
+      <c r="L115" s="37"/>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
@@ -6490,13 +6502,13 @@
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A127" s="38" t="s">
+      <c r="A127" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="B127" s="38"/>
-      <c r="C127" s="38"/>
-      <c r="D127" s="38"/>
-      <c r="E127" s="38"/>
+      <c r="B127" s="37"/>
+      <c r="C127" s="37"/>
+      <c r="D127" s="37"/>
+      <c r="E127" s="37"/>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
@@ -6626,15 +6638,15 @@
         <v>10</v>
       </c>
       <c r="C136" s="4">
-        <f t="shared" ref="C136:E136" si="6">_xlfn.MODE.SNGL(C129:C134)</f>
+        <f t="shared" ref="C136:E136" si="7">_xlfn.MODE.SNGL(C129:C134)</f>
         <v>4</v>
       </c>
       <c r="D136" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E136" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6644,18 +6656,18 @@
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="38" t="s">
+      <c r="A138" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="B138" s="38"/>
-      <c r="C138" s="38"/>
-      <c r="D138" s="38"/>
-      <c r="F138" s="38" t="s">
+      <c r="B138" s="37"/>
+      <c r="C138" s="37"/>
+      <c r="D138" s="37"/>
+      <c r="F138" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="G138" s="38"/>
-      <c r="H138" s="38"/>
-      <c r="I138" s="38"/>
+      <c r="G138" s="37"/>
+      <c r="H138" s="37"/>
+      <c r="I138" s="37"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
@@ -6722,7 +6734,7 @@
         <v>63</v>
       </c>
       <c r="D141" s="4" t="b">
-        <f t="shared" ref="D141:D148" si="7">OR(B141="Water",C141&gt;"60")</f>
+        <f t="shared" ref="D141:D148" si="8">OR(B141="Water",C141&gt;"60")</f>
         <v>0</v>
       </c>
       <c r="F141" s="4" t="s">
@@ -6735,7 +6747,7 @@
         <v>63</v>
       </c>
       <c r="I141" s="4" t="str">
-        <f t="shared" ref="I141:I148" si="8">IF(OR(G141="WATER",H141&gt;60),"Yes","No")</f>
+        <f t="shared" ref="I141:I148" si="9">IF(OR(G141="WATER",H141&gt;60),"Yes","No")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -6750,7 +6762,7 @@
         <v>83</v>
       </c>
       <c r="D142" s="4" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F142" s="4" t="s">
@@ -6763,7 +6775,7 @@
         <v>83</v>
       </c>
       <c r="I142" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6778,7 +6790,7 @@
         <v>43</v>
       </c>
       <c r="D143" s="4" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F143" s="4" t="s">
@@ -6791,7 +6803,7 @@
         <v>43</v>
       </c>
       <c r="I143" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>No</v>
       </c>
     </row>
@@ -6806,7 +6818,7 @@
         <v>58</v>
       </c>
       <c r="D144" s="4" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F144" s="4" t="s">
@@ -6819,7 +6831,7 @@
         <v>58</v>
       </c>
       <c r="I144" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>No</v>
       </c>
     </row>
@@ -6834,7 +6846,7 @@
         <v>78</v>
       </c>
       <c r="D145" s="4" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F145" s="4" t="s">
@@ -6847,7 +6859,7 @@
         <v>78</v>
       </c>
       <c r="I145" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6862,7 +6874,7 @@
         <v>65</v>
       </c>
       <c r="D146" s="4" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F146" s="4" t="s">
@@ -6875,7 +6887,7 @@
         <v>65</v>
       </c>
       <c r="I146" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6890,7 +6902,7 @@
         <v>80</v>
       </c>
       <c r="D147" s="4" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F147" s="4" t="s">
@@ -6903,7 +6915,7 @@
         <v>80</v>
       </c>
       <c r="I147" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6918,7 +6930,7 @@
         <v>100</v>
       </c>
       <c r="D148" s="4" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F148" s="4" t="s">
@@ -6931,7 +6943,7 @@
         <v>100</v>
       </c>
       <c r="I148" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Yes</v>
       </c>
     </row>
@@ -6941,23 +6953,23 @@
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A150" s="38" t="s">
+      <c r="A150" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="B150" s="38"/>
-      <c r="C150" s="38"/>
-      <c r="D150" s="38"/>
-      <c r="E150" s="38"/>
-      <c r="F150" s="38"/>
-      <c r="H150" s="38" t="s">
+      <c r="B150" s="37"/>
+      <c r="C150" s="37"/>
+      <c r="D150" s="37"/>
+      <c r="E150" s="37"/>
+      <c r="F150" s="37"/>
+      <c r="H150" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="I150" s="38"/>
-      <c r="J150" s="38"/>
-      <c r="K150" s="38"/>
-      <c r="L150" s="38"/>
-      <c r="M150" s="38"/>
-      <c r="N150" s="38"/>
+      <c r="I150" s="37"/>
+      <c r="J150" s="37"/>
+      <c r="K150" s="37"/>
+      <c r="L150" s="37"/>
+      <c r="M150" s="37"/>
+      <c r="N150" s="37"/>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
@@ -7554,14 +7566,14 @@
       </c>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B175" s="38" t="s">
+      <c r="B175" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="C175" s="38"/>
-      <c r="D175" s="38"/>
-      <c r="E175" s="38"/>
-      <c r="F175" s="38"/>
-      <c r="G175" s="38"/>
+      <c r="C175" s="37"/>
+      <c r="D175" s="37"/>
+      <c r="E175" s="37"/>
+      <c r="F175" s="37"/>
+      <c r="G175" s="37"/>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B176" s="4" t="s">
@@ -7623,7 +7635,7 @@
         <v>21</v>
       </c>
       <c r="G179" s="15">
-        <f t="shared" ref="G179:G180" si="9">SUMIF(C178:C186,C178,D178:D186)</f>
+        <f t="shared" ref="G179:G180" si="10">SUMIF(C178:C186,C178,D178:D186)</f>
         <v>930</v>
       </c>
     </row>
@@ -7641,7 +7653,7 @@
         <v>25</v>
       </c>
       <c r="G180" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>525</v>
       </c>
     </row>
@@ -7706,16 +7718,16 @@
       </c>
     </row>
     <row r="187" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B187" s="38" t="s">
+      <c r="B187" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="C187" s="38"/>
-      <c r="D187" s="38"/>
-      <c r="E187" s="38"/>
-      <c r="F187" s="38"/>
-      <c r="G187" s="38"/>
-      <c r="H187" s="38"/>
-      <c r="I187" s="38"/>
+      <c r="C187" s="37"/>
+      <c r="D187" s="37"/>
+      <c r="E187" s="37"/>
+      <c r="F187" s="37"/>
+      <c r="G187" s="37"/>
+      <c r="H187" s="37"/>
+      <c r="I187" s="37"/>
     </row>
     <row r="188" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B188" s="4" t="s">
@@ -7904,7 +7916,7 @@
         <v>1</v>
       </c>
       <c r="I195" s="15">
-        <f t="shared" ref="I195:I200" si="10">SUMIFS(D190:D202,C190:C202,G195,E190:E202,H195)</f>
+        <f t="shared" ref="I195:I200" si="11">SUMIFS(D190:D202,C190:C202,G195,E190:E202,H195)</f>
         <v>714</v>
       </c>
     </row>
@@ -7928,7 +7940,7 @@
         <v>2</v>
       </c>
       <c r="I196" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>534</v>
       </c>
     </row>
@@ -7952,7 +7964,7 @@
         <v>3</v>
       </c>
       <c r="I197" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -7976,7 +7988,7 @@
         <v>1</v>
       </c>
       <c r="I198" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>195</v>
       </c>
     </row>
@@ -8000,7 +8012,7 @@
         <v>2</v>
       </c>
       <c r="I199" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>600</v>
       </c>
     </row>
@@ -8024,7 +8036,7 @@
         <v>3</v>
       </c>
       <c r="I200" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>195</v>
       </c>
     </row>
@@ -8043,15 +8055,15 @@
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A203" s="38" t="s">
+      <c r="A203" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="B203" s="38"/>
-      <c r="C203" s="38"/>
-      <c r="D203" s="38"/>
-      <c r="E203" s="38"/>
-      <c r="F203" s="38"/>
-      <c r="G203" s="38"/>
+      <c r="B203" s="37"/>
+      <c r="C203" s="37"/>
+      <c r="D203" s="37"/>
+      <c r="E203" s="37"/>
+      <c r="F203" s="37"/>
+      <c r="G203" s="37"/>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="s">
@@ -8143,7 +8155,7 @@
       <c r="F208" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="G208" s="21" t="str">
+      <c r="G208" s="20" t="str">
         <f>VLOOKUP(G207,A205:E226,2,1)</f>
         <v xml:space="preserve">  Charizard</v>
       </c>
@@ -8431,12 +8443,12 @@
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A229" s="38" t="s">
+      <c r="A229" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="B229" s="38"/>
-      <c r="C229" s="38"/>
-      <c r="D229" s="38"/>
+      <c r="B229" s="37"/>
+      <c r="C229" s="37"/>
+      <c r="D229" s="37"/>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="4" t="s">
@@ -8463,7 +8475,7 @@
         <v>45</v>
       </c>
       <c r="D231" s="4" t="b">
-        <f t="shared" ref="D231:D239" si="11">_xlfn.XOR(B231="Fire", C231&lt;60)</f>
+        <f t="shared" ref="D231:D239" si="12">_xlfn.XOR(B231="Fire", C231&lt;60)</f>
         <v>1</v>
       </c>
     </row>
@@ -8478,7 +8490,7 @@
         <v>60</v>
       </c>
       <c r="D232" s="4" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -8493,7 +8505,7 @@
         <v>80</v>
       </c>
       <c r="D233" s="4" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -8508,7 +8520,7 @@
         <v>39</v>
       </c>
       <c r="D234" s="4" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -8523,7 +8535,7 @@
         <v>58</v>
       </c>
       <c r="D235" s="4" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -8538,7 +8550,7 @@
         <v>78</v>
       </c>
       <c r="D236" s="4" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -8553,7 +8565,7 @@
         <v>44</v>
       </c>
       <c r="D237" s="4" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -8568,7 +8580,7 @@
         <v>59</v>
       </c>
       <c r="D238" s="4" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -8583,7 +8595,7 @@
         <v>79</v>
       </c>
       <c r="D239" s="4" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -8594,6 +8606,15 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B175:G175"/>
+    <mergeCell ref="B187:I187"/>
+    <mergeCell ref="A203:G203"/>
+    <mergeCell ref="A229:D229"/>
+    <mergeCell ref="A127:E127"/>
+    <mergeCell ref="A138:D138"/>
+    <mergeCell ref="F138:I138"/>
+    <mergeCell ref="A150:F150"/>
+    <mergeCell ref="H150:N150"/>
     <mergeCell ref="A115:D115"/>
     <mergeCell ref="F115:L115"/>
     <mergeCell ref="A1:D1"/>
@@ -8607,15 +8628,6 @@
     <mergeCell ref="A88:H88"/>
     <mergeCell ref="A103:D103"/>
     <mergeCell ref="F103:I103"/>
-    <mergeCell ref="B175:G175"/>
-    <mergeCell ref="B187:I187"/>
-    <mergeCell ref="A203:G203"/>
-    <mergeCell ref="A229:D229"/>
-    <mergeCell ref="A127:E127"/>
-    <mergeCell ref="A138:D138"/>
-    <mergeCell ref="F138:I138"/>
-    <mergeCell ref="A150:F150"/>
-    <mergeCell ref="H150:N150"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8641,489 +8653,489 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="35" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="34" t="s">
         <v>209</v>
       </c>
-      <c r="D1" s="36">
+      <c r="D1" s="35">
         <v>45041</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="33" t="s">
         <v>208</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="33" t="s">
         <v>211</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="33" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="31">
         <v>10</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="30">
         <v>40</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="31">
         <f>PRODUCT(C4,D4)</f>
         <v>400</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="32">
         <f>IF(D4&gt;40,D4-40,0)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="36">
         <f xml:space="preserve"> 0.5*F4*C4</f>
         <v>0</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="31">
         <f>SUM(G4,E4)</f>
         <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="28">
         <v>15</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="27">
         <v>35</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="28">
         <f t="shared" ref="E5:E14" si="0">PRODUCT(C5,D5)</f>
         <v>525</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="29">
         <f t="shared" ref="F5:F14" si="1">IF(D5&gt;40,D5-40,0)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="37">
+      <c r="G5" s="36">
         <f t="shared" ref="G5:G14" si="2" xml:space="preserve"> 0.5*F5*C5</f>
         <v>0</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="28">
         <f t="shared" ref="H5:H14" si="3">SUM(G5,E5)</f>
         <v>525</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="31">
         <v>3.5</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="30">
         <v>30</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="31">
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G6" s="37">
+      <c r="G6" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H6" s="32">
+      <c r="H6" s="31">
         <f t="shared" si="3"/>
         <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="28">
         <v>20.100000000000001</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="27">
         <v>50</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="28">
         <f t="shared" si="0"/>
         <v>1005.0000000000001</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="29">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="G7" s="37">
+      <c r="G7" s="36">
         <f t="shared" si="2"/>
         <v>100.5</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="28">
         <f t="shared" si="3"/>
         <v>1105.5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="31">
         <v>5.75</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="30">
         <v>55</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <f t="shared" si="0"/>
         <v>316.25</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="32">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G8" s="37">
+      <c r="G8" s="36">
         <f t="shared" si="2"/>
         <v>43.125</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="31">
         <f t="shared" si="3"/>
         <v>359.375</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="28">
         <v>12</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="27">
         <v>45</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="28">
         <f t="shared" si="0"/>
         <v>540</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="29">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="36">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9" s="28">
         <f t="shared" si="3"/>
         <v>570</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <v>6.55</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="30">
         <v>25</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <f t="shared" si="0"/>
         <v>163.75</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G10" s="37">
+      <c r="G10" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="31">
         <f t="shared" si="3"/>
         <v>163.75</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="28">
         <v>30</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="27">
         <v>29</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="28">
         <f t="shared" si="0"/>
         <v>870</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G11" s="37">
+      <c r="G11" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H11" s="29">
+      <c r="H11" s="28">
         <f t="shared" si="3"/>
         <v>870</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="31">
         <v>75</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="30">
         <v>32</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="31">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G12" s="37">
+      <c r="G12" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="31">
         <f t="shared" si="3"/>
         <v>2400</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="28">
         <v>40</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="27">
         <v>44</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="28">
         <f t="shared" si="0"/>
         <v>1760</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="29">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G13" s="37">
+      <c r="G13" s="36">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="H13" s="29">
+      <c r="H13" s="28">
         <f t="shared" si="3"/>
         <v>1840</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="31">
         <v>25</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="30">
         <v>22</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="31">
         <f t="shared" si="0"/>
         <v>550</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G14" s="37">
+      <c r="G14" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H14" s="32">
+      <c r="H14" s="31">
         <f t="shared" si="3"/>
         <v>550</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="33" t="s">
         <v>204</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="32">
+      <c r="B16" s="30"/>
+      <c r="C16" s="31">
         <f t="shared" ref="C16:G16" si="4">MAX(C4:C14)</f>
         <v>75</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="31">
         <f t="shared" si="4"/>
         <v>55</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="31">
         <f t="shared" si="4"/>
         <v>2400</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="31">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="G16" s="32">
+      <c r="G16" s="31">
         <f t="shared" si="4"/>
         <v>100.5</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="31">
         <f>MAX(H4:H14)</f>
         <v>2400</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="33" t="s">
         <v>205</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="29">
+      <c r="B17" s="27"/>
+      <c r="C17" s="28">
         <f t="shared" ref="C17:G17" si="5">MIN(C4:C14)</f>
         <v>3.5</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="28">
         <f t="shared" si="5"/>
         <v>22</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="28">
         <f t="shared" si="5"/>
         <v>105</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G17" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H17" s="29">
+      <c r="H17" s="28">
         <f>MIN(H4:H14)</f>
         <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="33" t="s">
         <v>206</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="32">
+      <c r="B18" s="30"/>
+      <c r="C18" s="31">
         <f t="shared" ref="C18:G18" si="6">AVERAGE(C4:C14)</f>
         <v>22.081818181818178</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="31">
         <f t="shared" si="6"/>
         <v>37</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="31">
         <f t="shared" si="6"/>
         <v>785</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="31">
         <f t="shared" si="6"/>
         <v>3.0909090909090908</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="31">
         <f t="shared" si="6"/>
         <v>23.056818181818183</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="31">
         <f>AVERAGE(H4:H14)</f>
         <v>808.05681818181813</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="33" t="s">
         <v>207</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29">
+      <c r="B19" s="27"/>
+      <c r="C19" s="28">
         <f t="shared" ref="C19:G19" si="7">SUM(C4:C14)</f>
         <v>242.89999999999998</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="28">
         <f t="shared" si="7"/>
         <v>407</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="28">
         <f t="shared" si="7"/>
         <v>8635</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="28">
         <f t="shared" si="7"/>
         <v>34</v>
       </c>
-      <c r="G19" s="29">
+      <c r="G19" s="28">
         <f t="shared" si="7"/>
         <v>253.625</v>
       </c>
-      <c r="H19" s="29">
+      <c r="H19" s="28">
         <f>SUM(H4:H14)</f>
         <v>8888.625</v>
       </c>
@@ -9145,112 +9157,112 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.28515625" style="24" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="24"/>
+    <col min="1" max="1" width="5.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.28515625" style="23" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="25">
+      <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="25">
+      <c r="A3" s="24">
         <v>2</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="25">
+      <c r="A4" s="24">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="25">
+      <c r="A5" s="24">
         <v>4</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="25">
+      <c r="A6" s="24">
         <v>5</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="25">
+      <c r="A7" s="24">
         <v>6</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
+      <c r="A8" s="24">
         <v>7</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="25">
+      <c r="A9" s="24">
         <v>8</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="25">
+      <c r="A10" s="24">
         <v>9</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="25">
+      <c r="A11" s="24">
         <v>10</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="25">
+      <c r="A12" s="24">
         <v>11</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="25" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="25">
+      <c r="A13" s="24">
         <v>12</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="26" t="s">
         <v>176</v>
       </c>
     </row>

</xml_diff>